<commit_message>
Add palindrome and leetcode problem
</commit_message>
<xml_diff>
--- a/leetcode/LC-list.xlsx
+++ b/leetcode/LC-list.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jagaran" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Amazon" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="75 - blind" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Amazon!$A$1:$E$53</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="605">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -982,6 +983,864 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/word-search/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/KLlXCFG5TnA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use hash map to instantly check for difference value, map will add index of last occurrence of a num, don’t use same element twice;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/1pkOgXD63yU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find local min and search for local max, sliding window;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/3OamzN90kPg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains Duplicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/contains-duplicate/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hashset to get unique values in array, to check for duplicates easily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/bNvIQI2wAjk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product of Array Except Self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make two passes, first in-order, second in-reverse, to compute products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/5WZl3MMT0Eg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Subarray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pattern: prev subarray cant be negative, dynamic programming: compute max sum for each prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/lXVy6YWFcRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Product Subarray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-product-subarray/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dp: compute max and max-abs-val for each prefix subarr;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/nIVW4P8b1VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check if half of array is sorted in order to find pivot, arr is guaranteed to be in at most two sorted subarrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/U8XENwh8Oy8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at most two sorted halfs, mid will be apart of left sorted or right sorted, if target is in range of sorted portion then search it, otherwise search other half</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/jzZsG8n2R9A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort input, for each first element, find next two where -a = b+c, if a=prevA, skip a, if b=prevB skip b to elim duplicates; to find b,c use two pointers, left/right on remaining list;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/UuiTKBwPgAo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container With Most Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shrinking window, left/right initially at endpoints, shift the pointer with min height;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/gVUrDV4tZfY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of Two Integers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/sum-of-two-integers/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add bit by bit, be mindful of carry, after adding, if carry is still 1, then add it as well;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/5Km3utixwZs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of 1 Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/number-of-1-bits/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modulo, and dividing n; mod and div are expensive, to divide use bit shift, instead of mod to get 1's place use bitwise &amp; 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/RyBM56RIWrM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counting Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/counting-bits/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write out result for num=16 to figure out pattern; res[i] = res[i - offset], where offset is the biggest power of 2 &lt;= I;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/WnPLSRLSANE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/missing-number/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compute expected sum - real sum; xor n with each index and value;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/UcoN6UjAI64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/reverse-bits/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reverse each of 32 bits;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Y0lT9Fck7qI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climbing Stairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subproblem find (n-1) and (n-2), sum = n;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/H9bfqozjoqs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coin Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/coin-change/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">top-down: recursive dfs, for amount, branch for each coin, cache to store prev coin_count for each amount; bottom-up: compute coins for amount = 1, up until n, using for each coin (amount - coin), cache prev values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/cjWnW0hdF1Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-increasing-subsequence/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive: foreach num, get subseq with num and without num, only include num if prev was less, cache solution of each; dp=subseq length which must end with each num, curr num must be after a prev dp or by itself;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Ua0GhsJSlWM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-common-subsequence/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive: if first chars are equal find lcs of remaining of each, else max of: lcs of first and remain of 2nd and lcs of 2nd remain of first, cache result; nested forloop to compute the cache without recursion;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Sx9NNgInc3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word Break Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for each prefix, if prefix is in dict and wordbreak(remaining str)=True, then return True, cache result of wordbreak;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/GBKI9VSKdGg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combination Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/combination-sum/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualize the decision tree, base case is curSum = or &gt; target, each candidate can have children of itself or elements to right of it inorder to elim duplicate solutions;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/73r3KWiEvyk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House Robber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/house-robber/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for each num, get max of prev subarr, or num + prev subarr not including last element, store results of prev, and prev not including last element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/rWAJCfYYOvM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House Robber II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/house-robber-ii/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subarr = arr without first &amp; last, get max of subarr, then pick which of first/last should be added to it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/6aEyTjOwlJU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decode Ways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can cur char be decoded in one or two ways? Recursion -&gt; cache -&gt; iterative dp solution, a lot of edge cases to determine, 52, 31, 29, 10, 20 only decoded one way, 11, 26 decoded two ways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/IlEsdxuD4lY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Paths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work backwards from solution, store paths for each position in grid, to further optimize, we don’t store whole grid, only need to store prev row;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Yan0cv2cLy8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/jump-game/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visualize the recursive tree, cache solution for O(n) time/mem complexity, iterative is O(1) mem, just iterate backwards to see if element can reach goal node, if yes, then set it equal to goal node, continue;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/mQeF6bN8hMk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clone Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/clone-graph/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive dfs, hashmap for visited nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/EgI5nU9etnU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">build adjacentcy_list with edges, run dfs on each V, if while dfs on V we see V again, then loop exists, otherwise V isnt in a loop, 3 states= not visited, visited, still visiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/s-VkcjHqkGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Atlantic Water Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/pacific-atlantic-water-flow/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfs each cell, keep track of visited, and track which reach pac, atl; dfs on cells adjacent to pac, atl, find overlap of cells that are visited by both pac and atl cells;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/pV2kpPD66nE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreach cell, if cell is 1 and unvisited run dfs, increment cound and marking each contigous 1 as visited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/P6RZZMu_maU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-consecutive-sequence/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use bruteforce and try to optimize, consider the max subseq containing each num; add each num to hashset, for each num if num-1 doesn’t exist, count the consecutive nums after num, ie num+1; there is also a union-find solution;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/6kTZYvNNyps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alien Dictionary (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/alien-dictionary/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chars of a word not in order, the words are in order, find adjacency list of each unique char by iterating through adjacent words and finding first chars that are different, run topsort on graph and do loop detection;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/bXsUuownnoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph Valid Tree (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/graph-valid-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">union find, if union return false, loop exists, at end size must equal n, or its not connected; dfs to get size and check for loop, since each edge is double, before dfs on neighbor of N, remove N from neighbor list of neighbor;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/8f1XPm4WOUc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Connected Components in an Undirected Graph (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfs on each node that hasn’t been visited, increment component count, adjacency list; bfs and union find are possible;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/A8NUOmlwOlM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/insert-interval/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert new interval in order, then merge intervals; newinterval could only merge with one interval that comes before it, then add remaining intervals;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/44H3cEC2fFM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort each interval, overlapping intervals should be adjacent, iterate and build solution; also graph method, less efficient, more complicated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/nONCGxWoUfM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-overlapping Intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/non-overlapping-intervals/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instead of removing, count how max num of intervals you can include, sort intervals, dp to compute max intervals up until the i-th interval;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/PaJxqZVPhbg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting Rooms (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/meeting-rooms/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort intervals by start time, if second interval doesn’t overlap with first, then third def wont overlap with first;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/FdzJmTCVyJU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting Rooms II (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we care about the points in time where we are starting/ending a meeting, we already are given those, just separate start/end and traverse counting num of meetings going at these points in time; for each meeting check if a prev meeting has finished before curr started, using min heap;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/G0_I-ZF0S38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse a Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iterate through maintaining cur and prev; recursively reverse, return new head of list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/gBTe7lFR3vc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detect Cycle in a Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dict to remember visited nodes; two pointers at different speeds, if they meet there is loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/XIdigk956u0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert each node from one list into the other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/q5a5OiGbT6Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge K Sorted Lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">divied and conquer, merge lists, N totalnodes, k-lists, O(N*logk). For each list, find min val, insert it into list, use priorityQ to optimize finding min O(N*logk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/XVuQxVej6y8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Nth Node From End Of List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/remove-nth-node-from-end-of-list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use dummy node at head of list, compute len of list; two pointers, second has offset of n from first;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/S5bfdUTrKLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reorder List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/reorder-list/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reverse second half of list, then easily reorder it; non-optimal way is to store list in array;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/T41rL0L3Pnw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/set-matrix-zeroes/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use sets to keep track of all rows, cols to zero out, after, for each num if it is in a zero row or col then change it to 0; flag first cell in row, and col to mark row/col that needs to be zeroed;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/BJnMZNwUk1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spiral Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/spiral-matrix/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep track of visited cells; keep track of boundaries, layer-by-layer;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/fMSJSS7eO1w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotate Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/rotate-image/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate layer-by-layer, use that it's a square as advantage, rotate positions in reverse order, store a in temp, a = b, b = c, c = d, d = temp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/pfiQ_PS1g8E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfs on each cell, for each search remember visited cells, and remove cur visited cell right before you return from dfs;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/wiGpQwVHdE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliding window, if we see same char twice within curr window, shift start position;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/gqXU1UyA8pk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-repeating-character-replacement/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAY ATTENTION: limited to chars A-Z; for each capital char, check if it could create the longest repeating substr, use sliding window to optimize; check if windowlen=1 works, if yes, increment len, if not, shift window right;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/jSto0O4AJbM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Window Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need is num of unique char in T, HAVE is num of char we have valid count for, sliding window, move right until valid, if valid, increment left until invalid, to check validity keep track if the count of each unique char is satisfied;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/9UtInBqnCgA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Anagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hashmap to count each char in str1, decrement for str2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/vzdNOK2oB2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Anagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for each of 26 chars, use count of each char in each word as tuple for key in dict, value is the list of anagrams;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/WTzjTskDFMg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Parentheses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">push opening brace on stack, pop if matching close brace, at end if stack empty, return true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/jJXJ16kPFWg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Palindrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left, right pointers, update left and right until each points at alphanum, compare left and right, continue until left &gt;= right, don’t distinguish between upper/lowercase;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/XYQecbcd6_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreach char in str, consider it were the middle, consider if pali was odd or even;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/4RACzI5-du8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palindromic Substrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/palindromic-substrings/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same as longest palindromic string, each char in str as middle and expand outwards, do same for pali of even len; maybe read up on manachers alg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/B1k_sxOSgv8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encode and Decode Strings (Leetcode Premium)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/encode-and-decode-strings/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store length of str before each string and delimiter like '#';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/hTM3phVI6YQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive dfs to find max-depth of subtrees; iterative bfs to count number of levels in tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/vRbbcKXCxOw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive dfs on both trees at the same time; iterative bfs compare each level of both trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/OnSn2XEQ4MY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invert/Flip Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive dfs to invert subtrees; bfs to invert levels, use collections.deque; iterative dfs is easy with stack if doing pre-order traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Hr5cWUld4vU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helper returns maxpathsum without splitting branches, inside helper we also update maxSum by computing maxpathsum WITH a split;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/6ZnyEApgFYg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iterative bfs, add prev level which doesn't have any nulls to the result;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/u4JAi2JJhI8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serialize and Deserialize Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/serialize-and-deserialize-binary-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfs every single non-null node is added to string, and it's children are added too, even if they're null, deserialize by adding each non-null node to queue, deque node, it's children are next two nodes in string;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/E36O5SWp-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traverse s to check if any subtree in s equals t; merkle hashing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/ihj4IQGZ2zc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first element in pre-order is root, elements left of root in in-order are left subtree, right of root are right subtree, recursively build subtrees;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/s6ATEkipzow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trick is use built in python min/max values float("inf"), "-inf", as parameters; iterative in-order traversal, check each val is greater than prev;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/5LUXSvjmGCw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-optimal store tree in sorted array; iterative dfs in-order and return the kth element processed, go left until null, pop, go right once;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/gs2LMfuOR9k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lowest Common Ancestor of BST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare p, q values to curr node, base case: one is in left, other in right subtree, then curr is lca;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/oobqoCJlHA0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node has children characters, and bool if its an ending character, node DOESN’T have or need char, since root node doesn’t have a char, only children;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/BTf05gs_8iU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add and Search Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/add-and-search-word-data-structure-design/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if char = "." run search for remaining portion of word on all of curr nodes children;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/asbcE9mZz_U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word Search II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trick: I though use trie to store the grid, reverse thinking, instead store dictionary words, dfs on each cell, check if cell's char exists as child of root node in trie, if it does, update currNode, and check neighbors, a word could exist multiple times in grid, so don’t add duplicates;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we always want the min of the current frontier, we can store frontier in heap of size k for efficient pop/push; divide and conquer merging lists;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/YPTqKIgVk-k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minheap that’s kept at size k, if its bigger than k pop the min, by the end it should be left with k largest;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/itmhHWaHupI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Median from Data Stream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintain curr median, and all num greater than med in a minHeap, and all num less than med in a maxHeap, after every insertion update median depending on odd/even num of elements;</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1935,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1086,6 +1945,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -1124,7 +1989,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1167,6 +2032,18 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1215,7 +2092,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFE8F2A1"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -1251,16 +2128,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.22"/>
@@ -1291,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="n">
         <v>1</v>
@@ -1304,7 +2181,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="n">
         <v>2</v>
@@ -1317,7 +2194,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="n">
         <v>3</v>
@@ -1330,7 +2207,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="n">
         <v>9</v>
@@ -1343,7 +2220,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="n">
         <v>11</v>
@@ -1356,7 +2233,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="n">
         <v>14</v>
@@ -1369,7 +2246,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="n">
         <v>17</v>
@@ -1382,7 +2259,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="n">
         <v>19</v>
@@ -1395,7 +2272,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="n">
         <v>20</v>
@@ -1408,7 +2285,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="n">
         <v>21</v>
@@ -1438,7 +2315,7 @@
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="n">
         <v>24</v>
@@ -1451,7 +2328,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="n">
         <v>26</v>
@@ -1464,7 +2341,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="n">
         <v>27</v>
@@ -1477,7 +2354,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="n">
         <v>31</v>
@@ -1490,7 +2367,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="n">
         <v>32</v>
@@ -1507,7 +2384,7 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="n">
         <v>33</v>
@@ -1520,7 +2397,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="n">
         <v>34</v>
@@ -1533,7 +2410,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="n">
         <v>35</v>
@@ -1546,7 +2423,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="n">
         <v>36</v>
@@ -1559,7 +2436,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="n">
         <v>38</v>
@@ -1571,7 +2448,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="n">
         <v>39</v>
@@ -1584,7 +2461,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="n">
         <v>40</v>
@@ -1597,7 +2474,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="n">
         <v>41</v>
@@ -1610,7 +2487,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="n">
         <v>42</v>
@@ -1644,7 +2521,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="n">
         <v>46</v>
@@ -1657,7 +2534,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="n">
         <v>47</v>
@@ -1670,7 +2547,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="n">
         <v>49</v>
@@ -1719,7 +2596,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="n">
         <v>56</v>
@@ -1732,7 +2609,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="n">
         <v>58</v>
@@ -1745,7 +2622,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="n">
         <v>61</v>
@@ -1809,7 +2686,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="3" t="n">
         <v>66</v>
@@ -1822,7 +2699,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="3" t="n">
         <v>67</v>
@@ -1852,7 +2729,7 @@
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="3" t="n">
         <v>74</v>
@@ -1865,7 +2742,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="3" t="n">
         <v>77</v>
@@ -1878,7 +2755,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="3" t="n">
         <v>78</v>
@@ -1891,7 +2768,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="3" t="n">
         <v>79</v>
@@ -1904,7 +2781,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="3" t="n">
         <v>80</v>
@@ -1917,7 +2794,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="3" t="n">
         <v>82</v>
@@ -1930,7 +2807,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="3" t="n">
         <v>83</v>
@@ -1943,7 +2820,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="3" t="n">
         <v>86</v>
@@ -1956,7 +2833,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="3" t="n">
         <v>90</v>
@@ -1986,7 +2863,7 @@
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="3" t="n">
         <v>92</v>
@@ -1999,7 +2876,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="3" t="n">
         <v>94</v>
@@ -2046,7 +2923,7 @@
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="3" t="n">
         <v>98</v>
@@ -2059,7 +2936,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="n">
         <v>99</v>
@@ -2072,7 +2949,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="3" t="n">
         <v>100</v>
@@ -2085,7 +2962,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="3" t="n">
         <v>101</v>
@@ -2098,7 +2975,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="n">
         <v>102</v>
@@ -2111,7 +2988,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="3" t="n">
         <v>104</v>
@@ -2124,7 +3001,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="3" t="n">
         <v>107</v>
@@ -2137,7 +3014,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="n">
         <v>108</v>
@@ -2150,7 +3027,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="3" t="n">
         <v>110</v>
@@ -2163,7 +3040,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="3" t="n">
         <v>111</v>
@@ -2176,7 +3053,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="2"/>
       <c r="B66" s="3" t="n">
         <v>112</v>
@@ -2189,7 +3066,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="3" t="n">
         <v>113</v>
@@ -2202,7 +3079,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
       <c r="B68" s="3" t="n">
         <v>114</v>
@@ -2215,7 +3092,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
       <c r="B69" s="3" t="n">
         <v>116</v>
@@ -2228,7 +3105,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
       <c r="B70" s="3" t="n">
         <v>117</v>
@@ -2311,7 +3188,7 @@
       </c>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="3" t="n">
         <v>124</v>
@@ -2328,7 +3205,7 @@
       </c>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="3" t="n">
         <v>125</v>
@@ -2341,7 +3218,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="3" t="n">
         <v>129</v>
@@ -2354,7 +3231,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="3" t="n">
         <v>136</v>
@@ -2367,7 +3244,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
       <c r="B79" s="3" t="n">
         <v>138</v>
@@ -2380,7 +3257,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="2"/>
       <c r="B80" s="3" t="n">
         <v>155</v>
@@ -2393,7 +3270,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2"/>
       <c r="B81" s="3" t="n">
         <v>162</v>
@@ -2406,7 +3283,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2"/>
       <c r="B82" s="3" t="n">
         <v>169</v>
@@ -2419,7 +3296,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="7"/>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2"/>
       <c r="B83" s="3" t="n">
         <v>198</v>
@@ -2432,7 +3309,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2"/>
       <c r="B84" s="3" t="n">
         <v>199</v>
@@ -2445,7 +3322,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2"/>
       <c r="B85" s="3" t="n">
         <v>200</v>
@@ -2458,7 +3335,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="2"/>
       <c r="B86" s="3" t="n">
         <v>203</v>
@@ -2471,7 +3348,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="2"/>
       <c r="B87" s="3" t="n">
         <v>206</v>
@@ -2484,7 +3361,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="2"/>
       <c r="B88" s="3" t="n">
         <v>209</v>
@@ -2514,7 +3391,7 @@
       </c>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="2"/>
       <c r="B90" s="3" t="n">
         <v>215</v>
@@ -2527,7 +3404,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="2"/>
       <c r="B91" s="3" t="n">
         <v>217</v>
@@ -2540,7 +3417,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="7"/>
     </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="2"/>
       <c r="B92" s="3" t="n">
         <v>219</v>
@@ -2553,7 +3430,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="2"/>
       <c r="B93" s="3" t="n">
         <v>222</v>
@@ -2566,7 +3443,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="2"/>
       <c r="B94" s="3" t="n">
         <v>226</v>
@@ -2579,7 +3456,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="2"/>
       <c r="B95" s="3" t="n">
         <v>230</v>
@@ -2592,7 +3469,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2"/>
       <c r="B96" s="3" t="n">
         <v>235</v>
@@ -2605,7 +3482,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
       <c r="B97" s="3" t="n">
         <v>236</v>
@@ -2618,7 +3495,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
       <c r="B98" s="3" t="n">
         <v>237</v>
@@ -2630,7 +3507,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2"/>
       <c r="B99" s="3" t="n">
         <v>238</v>
@@ -2643,7 +3520,7 @@
       <c r="F99" s="6"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2"/>
       <c r="B100" s="3" t="n">
         <v>240</v>
@@ -2656,7 +3533,7 @@
       <c r="F100" s="6"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2"/>
       <c r="B101" s="3" t="n">
         <v>242</v>
@@ -2669,7 +3546,7 @@
       <c r="F101" s="6"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2"/>
       <c r="B102" s="3" t="n">
         <v>257</v>
@@ -2682,7 +3559,7 @@
       <c r="F102" s="6"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="2"/>
       <c r="B103" s="3" t="n">
         <v>263</v>
@@ -2694,7 +3571,7 @@
       <c r="F103" s="6"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="2"/>
       <c r="B104" s="3" t="n">
         <v>268</v>
@@ -2707,7 +3584,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="2"/>
       <c r="B105" s="3" t="n">
         <v>278</v>
@@ -2737,7 +3614,7 @@
       </c>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2"/>
       <c r="B107" s="3" t="n">
         <v>283</v>
@@ -2750,7 +3627,7 @@
       <c r="F107" s="6"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="2"/>
       <c r="B108" s="3" t="n">
         <v>306</v>
@@ -2779,7 +3656,7 @@
       </c>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="2"/>
       <c r="B110" s="3" t="n">
         <v>328</v>
@@ -2792,7 +3669,7 @@
       <c r="F110" s="6"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="2"/>
       <c r="B111" s="3" t="n">
         <v>331</v>
@@ -2805,7 +3682,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="2"/>
       <c r="B112" s="3" t="n">
         <v>345</v>
@@ -2817,7 +3694,7 @@
       <c r="F112" s="6"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="2"/>
       <c r="B113" s="3" t="n">
         <v>380</v>
@@ -2830,7 +3707,7 @@
       <c r="F113" s="6"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="2"/>
       <c r="B114" s="3" t="n">
         <v>386</v>
@@ -2842,7 +3719,7 @@
       <c r="F114" s="6"/>
       <c r="G114" s="7"/>
     </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="2"/>
       <c r="B115" s="3" t="n">
         <v>387</v>
@@ -2874,7 +3751,7 @@
       </c>
       <c r="G116" s="7"/>
     </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="2"/>
       <c r="B117" s="3" t="n">
         <v>403</v>
@@ -2891,7 +3768,7 @@
       </c>
       <c r="G117" s="7"/>
     </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="2"/>
       <c r="B118" s="3" t="n">
         <v>404</v>
@@ -2904,7 +3781,7 @@
       <c r="F118" s="6"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="2"/>
       <c r="B119" s="3" t="n">
         <v>409</v>
@@ -2917,7 +3794,7 @@
       <c r="F119" s="6"/>
       <c r="G119" s="7"/>
     </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="2"/>
       <c r="B120" s="3" t="n">
         <v>412</v>
@@ -2930,7 +3807,7 @@
       <c r="F120" s="6"/>
       <c r="G120" s="7"/>
     </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="2"/>
       <c r="B121" s="3" t="n">
         <v>414</v>
@@ -2943,7 +3820,7 @@
       <c r="F121" s="6"/>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="2"/>
       <c r="B122" s="3" t="n">
         <v>419</v>
@@ -2955,7 +3832,7 @@
       <c r="F122" s="6"/>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="2"/>
       <c r="B123" s="3" t="n">
         <v>430</v>
@@ -2968,7 +3845,7 @@
       <c r="F123" s="6"/>
       <c r="G123" s="7"/>
     </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="2"/>
       <c r="B124" s="3" t="n">
         <v>437</v>
@@ -2981,7 +3858,7 @@
       <c r="F124" s="6"/>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="2"/>
       <c r="B125" s="3" t="n">
         <v>443</v>
@@ -2993,7 +3870,7 @@
       <c r="F125" s="6"/>
       <c r="G125" s="7"/>
     </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="2"/>
       <c r="B126" s="3" t="n">
         <v>448</v>
@@ -3006,7 +3883,7 @@
       <c r="F126" s="6"/>
       <c r="G126" s="7"/>
     </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="2"/>
       <c r="B127" s="3" t="n">
         <v>463</v>
@@ -3036,7 +3913,7 @@
       </c>
       <c r="G128" s="7"/>
     </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="2"/>
       <c r="B129" s="3" t="n">
         <v>501</v>
@@ -3048,7 +3925,7 @@
       <c r="F129" s="6"/>
       <c r="G129" s="7"/>
     </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="2"/>
       <c r="B130" s="3" t="n">
         <v>513</v>
@@ -3060,7 +3937,7 @@
       <c r="F130" s="6"/>
       <c r="G130" s="7"/>
     </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="2"/>
       <c r="B131" s="3" t="n">
         <v>515</v>
@@ -3072,7 +3949,7 @@
       <c r="F131" s="6"/>
       <c r="G131" s="7"/>
     </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="2"/>
       <c r="B132" s="3" t="n">
         <v>524</v>
@@ -3085,7 +3962,7 @@
       <c r="F132" s="6"/>
       <c r="G132" s="7"/>
     </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="2"/>
       <c r="B133" s="3" t="n">
         <v>530</v>
@@ -3097,7 +3974,7 @@
       <c r="F133" s="6"/>
       <c r="G133" s="7"/>
     </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="2"/>
       <c r="B134" s="3" t="n">
         <v>532</v>
@@ -3110,7 +3987,7 @@
       <c r="F134" s="6"/>
       <c r="G134" s="7"/>
     </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="2"/>
       <c r="B135" s="3" t="n">
         <v>538</v>
@@ -3123,7 +4000,7 @@
       <c r="F135" s="6"/>
       <c r="G135" s="7"/>
     </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="2"/>
       <c r="B136" s="3" t="n">
         <v>543</v>
@@ -3136,7 +4013,7 @@
       <c r="F136" s="6"/>
       <c r="G136" s="7"/>
     </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="2"/>
       <c r="B137" s="3" t="n">
         <v>547</v>
@@ -3149,7 +4026,7 @@
       <c r="F137" s="6"/>
       <c r="G137" s="7"/>
     </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="2"/>
       <c r="B138" s="3" t="n">
         <v>559</v>
@@ -3162,7 +4039,7 @@
       <c r="F138" s="6"/>
       <c r="G138" s="7"/>
     </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="2"/>
       <c r="B139" s="3" t="n">
         <v>566</v>
@@ -3175,7 +4052,7 @@
       <c r="F139" s="6"/>
       <c r="G139" s="7"/>
     </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="2"/>
       <c r="B140" s="3" t="n">
         <v>572</v>
@@ -3187,7 +4064,7 @@
       <c r="F140" s="6"/>
       <c r="G140" s="7"/>
     </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="2"/>
       <c r="B141" s="3" t="n">
         <v>617</v>
@@ -3200,7 +4077,7 @@
       <c r="F141" s="6"/>
       <c r="G141" s="7"/>
     </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="2"/>
       <c r="B142" s="3" t="n">
         <v>623</v>
@@ -3213,7 +4090,7 @@
       <c r="F142" s="6"/>
       <c r="G142" s="7"/>
     </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="2"/>
       <c r="B143" s="3" t="n">
         <v>637</v>
@@ -3243,7 +4120,7 @@
       </c>
       <c r="G144" s="7"/>
     </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="2"/>
       <c r="B145" s="3" t="n">
         <v>653</v>
@@ -3256,7 +4133,7 @@
       <c r="F145" s="6"/>
       <c r="G145" s="7"/>
     </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="2"/>
       <c r="B146" s="3" t="n">
         <v>654</v>
@@ -3269,7 +4146,7 @@
       <c r="F146" s="6"/>
       <c r="G146" s="7"/>
     </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="2"/>
       <c r="B147" s="3" t="n">
         <v>662</v>
@@ -3282,7 +4159,7 @@
       <c r="F147" s="6"/>
       <c r="G147" s="7"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="2"/>
       <c r="B148" s="3" t="n">
         <v>669</v>
@@ -3295,7 +4172,7 @@
       <c r="F148" s="6"/>
       <c r="G148" s="7"/>
     </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="2"/>
       <c r="B149" s="3" t="n">
         <v>671</v>
@@ -3308,7 +4185,7 @@
       <c r="F149" s="6"/>
       <c r="G149" s="7"/>
     </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="2"/>
       <c r="B150" s="3" t="n">
         <v>674</v>
@@ -3321,7 +4198,7 @@
       <c r="F150" s="6"/>
       <c r="G150" s="7"/>
     </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="2"/>
       <c r="B151" s="3" t="n">
         <v>680</v>
@@ -3333,7 +4210,7 @@
       <c r="F151" s="6"/>
       <c r="G151" s="7"/>
     </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="2"/>
       <c r="B152" s="3" t="n">
         <v>687</v>
@@ -3346,7 +4223,7 @@
       <c r="F152" s="6"/>
       <c r="G152" s="7"/>
     </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="2"/>
       <c r="B153" s="3" t="n">
         <v>695</v>
@@ -3359,7 +4236,7 @@
       <c r="F153" s="6"/>
       <c r="G153" s="7"/>
     </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="2"/>
       <c r="B154" s="3" t="n">
         <v>700</v>
@@ -3372,7 +4249,7 @@
       <c r="F154" s="6"/>
       <c r="G154" s="7"/>
     </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="2"/>
       <c r="B155" s="3" t="n">
         <v>725</v>
@@ -3385,7 +4262,7 @@
       <c r="F155" s="6"/>
       <c r="G155" s="7"/>
     </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="2"/>
       <c r="B156" s="3" t="n">
         <v>733</v>
@@ -3415,7 +4292,7 @@
       </c>
       <c r="G157" s="7"/>
     </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="2"/>
       <c r="B158" s="3" t="n">
         <v>784</v>
@@ -3428,7 +4305,7 @@
       <c r="F158" s="6"/>
       <c r="G158" s="7"/>
     </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="2"/>
       <c r="B159" s="3" t="n">
         <v>814</v>
@@ -3441,7 +4318,7 @@
       <c r="F159" s="6"/>
       <c r="G159" s="7"/>
     </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="2"/>
       <c r="B160" s="3" t="n">
         <v>852</v>
@@ -3454,7 +4331,7 @@
       <c r="F160" s="6"/>
       <c r="G160" s="7"/>
     </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="2"/>
       <c r="B161" s="3" t="n">
         <v>863</v>
@@ -3467,7 +4344,7 @@
       <c r="F161" s="6"/>
       <c r="G161" s="7"/>
     </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="2"/>
       <c r="B162" s="3" t="n">
         <v>865</v>
@@ -3480,7 +4357,7 @@
       <c r="F162" s="6"/>
       <c r="G162" s="7"/>
     </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="2"/>
       <c r="B163" s="3" t="n">
         <v>872</v>
@@ -3493,7 +4370,7 @@
       <c r="F163" s="6"/>
       <c r="G163" s="7"/>
     </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="2"/>
       <c r="B164" s="3" t="n">
         <v>876</v>
@@ -3506,7 +4383,7 @@
       <c r="F164" s="6"/>
       <c r="G164" s="7"/>
     </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="2"/>
       <c r="B165" s="3" t="n">
         <v>897</v>
@@ -3519,7 +4396,7 @@
       <c r="F165" s="6"/>
       <c r="G165" s="7"/>
     </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="2"/>
       <c r="B166" s="3" t="n">
         <v>904</v>
@@ -3531,7 +4408,7 @@
       <c r="F166" s="6"/>
       <c r="G166" s="7"/>
     </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="2"/>
       <c r="B167" s="3" t="n">
         <v>905</v>
@@ -3544,7 +4421,7 @@
       <c r="F167" s="6"/>
       <c r="G167" s="7"/>
     </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="2"/>
       <c r="B168" s="3" t="n">
         <v>908</v>
@@ -3556,7 +4433,7 @@
       <c r="F168" s="6"/>
       <c r="G168" s="7"/>
     </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="2"/>
       <c r="B169" s="3" t="n">
         <v>917</v>
@@ -3569,7 +4446,7 @@
       <c r="F169" s="6"/>
       <c r="G169" s="7"/>
     </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="2"/>
       <c r="B170" s="3" t="n">
         <v>921</v>
@@ -3582,7 +4459,7 @@
       <c r="F170" s="6"/>
       <c r="G170" s="7"/>
     </row>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="2"/>
       <c r="B171" s="3" t="n">
         <v>938</v>
@@ -3595,7 +4472,7 @@
       <c r="F171" s="6"/>
       <c r="G171" s="7"/>
     </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="2"/>
       <c r="B172" s="3" t="n">
         <v>941</v>
@@ -3608,7 +4485,7 @@
       <c r="F172" s="6"/>
       <c r="G172" s="7"/>
     </row>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="2"/>
       <c r="B173" s="3" t="n">
         <v>951</v>
@@ -3621,7 +4498,7 @@
       <c r="F173" s="6"/>
       <c r="G173" s="7"/>
     </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="2"/>
       <c r="B174" s="3" t="n">
         <v>953</v>
@@ -3634,7 +4511,7 @@
       <c r="F174" s="6"/>
       <c r="G174" s="7"/>
     </row>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="2"/>
       <c r="B175" s="3" t="n">
         <v>958</v>
@@ -3646,7 +4523,7 @@
       <c r="F175" s="6"/>
       <c r="G175" s="7"/>
     </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="2"/>
       <c r="B176" s="3" t="n">
         <v>965</v>
@@ -3659,7 +4536,7 @@
       <c r="F176" s="6"/>
       <c r="G176" s="7"/>
     </row>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="2"/>
       <c r="B177" s="3" t="n">
         <v>977</v>
@@ -3672,7 +4549,7 @@
       <c r="F177" s="6"/>
       <c r="G177" s="7"/>
     </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="2"/>
       <c r="B178" s="3" t="n">
         <v>980</v>
@@ -3685,7 +4562,7 @@
       <c r="F178" s="6"/>
       <c r="G178" s="7"/>
     </row>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="2"/>
       <c r="B179" s="3" t="n">
         <v>988</v>
@@ -3698,7 +4575,7 @@
       <c r="F179" s="6"/>
       <c r="G179" s="7"/>
     </row>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="2"/>
       <c r="B180" s="3" t="n">
         <v>993</v>
@@ -3711,7 +4588,7 @@
       <c r="F180" s="6"/>
       <c r="G180" s="7"/>
     </row>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="2"/>
       <c r="B181" s="3" t="n">
         <v>994</v>
@@ -3724,7 +4601,7 @@
       <c r="F181" s="6"/>
       <c r="G181" s="7"/>
     </row>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="2"/>
       <c r="B182" s="3" t="n">
         <v>998</v>
@@ -3736,7 +4613,7 @@
       <c r="F182" s="6"/>
       <c r="G182" s="7"/>
     </row>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="2"/>
       <c r="B183" s="3" t="n">
         <v>1005</v>
@@ -3748,7 +4625,7 @@
       <c r="F183" s="6"/>
       <c r="G183" s="7"/>
     </row>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="2"/>
       <c r="B184" s="3" t="n">
         <v>1038</v>
@@ -3760,7 +4637,7 @@
       <c r="F184" s="6"/>
       <c r="G184" s="7"/>
     </row>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="2"/>
       <c r="B185" s="3" t="n">
         <v>1079</v>
@@ -3772,7 +4649,7 @@
       <c r="F185" s="6"/>
       <c r="G185" s="7"/>
     </row>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="2"/>
       <c r="B186" s="3" t="n">
         <v>1095</v>
@@ -3784,7 +4661,7 @@
       <c r="F186" s="6"/>
       <c r="G186" s="7"/>
     </row>
-    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="2"/>
       <c r="B187" s="3" t="n">
         <v>1104</v>
@@ -3796,7 +4673,7 @@
       <c r="F187" s="6"/>
       <c r="G187" s="7"/>
     </row>
-    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="2"/>
       <c r="B188" s="3" t="n">
         <v>1110</v>
@@ -3808,7 +4685,7 @@
       <c r="F188" s="6"/>
       <c r="G188" s="7"/>
     </row>
-    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="2"/>
       <c r="B189" s="3" t="n">
         <v>1161</v>
@@ -3821,7 +4698,7 @@
       <c r="F189" s="6"/>
       <c r="G189" s="7"/>
     </row>
-    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="2"/>
       <c r="B190" s="3" t="n">
         <v>1219</v>
@@ -3833,7 +4710,7 @@
       <c r="F190" s="6"/>
       <c r="G190" s="7"/>
     </row>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="2"/>
       <c r="B191" s="3" t="n">
         <v>1232</v>
@@ -3845,7 +4722,7 @@
       <c r="F191" s="6"/>
       <c r="G191" s="7"/>
     </row>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="2"/>
       <c r="B192" s="3" t="n">
         <v>1249</v>
@@ -3858,7 +4735,7 @@
       <c r="F192" s="6"/>
       <c r="G192" s="7"/>
     </row>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="2"/>
       <c r="B193" s="3" t="n">
         <v>1254</v>
@@ -3870,7 +4747,7 @@
       <c r="F193" s="6"/>
       <c r="G193" s="7"/>
     </row>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="2"/>
       <c r="B194" s="3" t="n">
         <v>1290</v>
@@ -3883,7 +4760,7 @@
       <c r="F194" s="6"/>
       <c r="G194" s="7"/>
     </row>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="2"/>
       <c r="B195" s="3" t="n">
         <v>1299</v>
@@ -3895,7 +4772,7 @@
       <c r="F195" s="6"/>
       <c r="G195" s="7"/>
     </row>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="2"/>
       <c r="B196" s="3" t="n">
         <v>1302</v>
@@ -3908,7 +4785,7 @@
       <c r="F196" s="6"/>
       <c r="G196" s="7"/>
     </row>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="2"/>
       <c r="B197" s="3" t="n">
         <v>1315</v>
@@ -3920,7 +4797,7 @@
       <c r="F197" s="6"/>
       <c r="G197" s="7"/>
     </row>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="2"/>
       <c r="B198" s="3" t="n">
         <v>1325</v>
@@ -3932,7 +4809,7 @@
       <c r="F198" s="6"/>
       <c r="G198" s="7"/>
     </row>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="2"/>
       <c r="B199" s="3" t="n">
         <v>1351</v>
@@ -3944,7 +4821,7 @@
       <c r="F199" s="6"/>
       <c r="G199" s="7"/>
     </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="2"/>
       <c r="B200" s="3" t="n">
         <v>1372</v>
@@ -3956,7 +4833,7 @@
       <c r="F200" s="6"/>
       <c r="G200" s="7"/>
     </row>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="2"/>
       <c r="B201" s="3" t="n">
         <v>1373</v>
@@ -3968,7 +4845,7 @@
       <c r="F201" s="6"/>
       <c r="G201" s="7"/>
     </row>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="2"/>
       <c r="B202" s="3" t="n">
         <v>1376</v>
@@ -3980,7 +4857,7 @@
       <c r="F202" s="6"/>
       <c r="G202" s="7"/>
     </row>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="2"/>
       <c r="B203" s="3" t="n">
         <v>1379</v>
@@ -3993,7 +4870,7 @@
       <c r="F203" s="6"/>
       <c r="G203" s="7"/>
     </row>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="2"/>
       <c r="B204" s="3" t="n">
         <v>1382</v>
@@ -4005,7 +4882,7 @@
       <c r="F204" s="6"/>
       <c r="G204" s="7"/>
     </row>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="2"/>
       <c r="B205" s="3" t="n">
         <v>1403</v>
@@ -4017,7 +4894,7 @@
       <c r="F205" s="6"/>
       <c r="G205" s="7"/>
     </row>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="2"/>
       <c r="B206" s="3" t="n">
         <v>1416</v>
@@ -4033,7 +4910,7 @@
       </c>
       <c r="G206" s="7"/>
     </row>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="2"/>
       <c r="B207" s="3" t="n">
         <v>1417</v>
@@ -4045,7 +4922,7 @@
       <c r="F207" s="6"/>
       <c r="G207" s="7"/>
     </row>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="2"/>
       <c r="B208" s="3" t="n">
         <v>1437</v>
@@ -4058,7 +4935,7 @@
       <c r="F208" s="6"/>
       <c r="G208" s="7"/>
     </row>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="2"/>
       <c r="B209" s="3" t="n">
         <v>1448</v>
@@ -4071,7 +4948,7 @@
       <c r="F209" s="6"/>
       <c r="G209" s="7"/>
     </row>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="2"/>
       <c r="B210" s="3" t="n">
         <v>1464</v>
@@ -4083,7 +4960,7 @@
       <c r="F210" s="6"/>
       <c r="G210" s="7"/>
     </row>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="2"/>
       <c r="B211" s="3" t="n">
         <v>1563</v>
@@ -4099,7 +4976,7 @@
       </c>
       <c r="G211" s="7"/>
     </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="2"/>
       <c r="B212" s="3" t="n">
         <v>1573</v>
@@ -4111,7 +4988,7 @@
       <c r="F212" s="6"/>
       <c r="G212" s="7"/>
     </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="2"/>
       <c r="B213" s="3" t="n">
         <v>1609</v>
@@ -4123,7 +5000,7 @@
       <c r="F213" s="6"/>
       <c r="G213" s="7"/>
     </row>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="2"/>
       <c r="B214" s="3" t="n">
         <v>1614</v>
@@ -4135,7 +5012,7 @@
       <c r="F214" s="6"/>
       <c r="G214" s="7"/>
     </row>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="2"/>
       <c r="B215" s="3" t="n">
         <v>1647</v>
@@ -4147,7 +5024,7 @@
       <c r="F215" s="6"/>
       <c r="G215" s="7"/>
     </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="2"/>
       <c r="B216" s="3" t="n">
         <v>1669</v>
@@ -4159,7 +5036,7 @@
       <c r="F216" s="6"/>
       <c r="G216" s="7"/>
     </row>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="2"/>
       <c r="B217" s="3" t="n">
         <v>1710</v>
@@ -4172,7 +5049,7 @@
       <c r="F217" s="6"/>
       <c r="G217" s="7"/>
     </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="2"/>
       <c r="B218" s="3" t="n">
         <v>1721</v>
@@ -4185,7 +5062,7 @@
       <c r="F218" s="6"/>
       <c r="G218" s="7"/>
     </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="2"/>
       <c r="B219" s="3" t="n">
         <v>1827</v>
@@ -4197,7 +5074,7 @@
       <c r="F219" s="6"/>
       <c r="G219" s="7"/>
     </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="2"/>
       <c r="B220" s="3" t="n">
         <v>1877</v>
@@ -4990,7 +5867,19 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="B1:F220"/>
+  <autoFilter ref="B1:F220">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="DP"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Easy"/>
+        <filter val="Medium"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Two Sum    "/>
     <hyperlink ref="C3" r:id="rId2" display="Add Two Numbers    "/>
@@ -5230,11 +6119,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.44"/>
@@ -7180,4 +8069,1498 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E77"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="89.46"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="12" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="24.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="22.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="21.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="20.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="26.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="22.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="30.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="26.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="26.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="26.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="22.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="24.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="22.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="18.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>514</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>521</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="22.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="13" t="s">
+        <v>527</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>528</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>532</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13" t="s">
+        <v>534</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>535</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>538</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="13" t="s">
+        <v>545</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="13" t="s">
+        <v>549</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>551</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="24.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>554</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>555</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>558</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="13" t="s">
+        <v>560</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>562</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>566</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="26.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13" t="s">
+        <v>568</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>569</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="26.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>572</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="26.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="13" t="s">
+        <v>574</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="32.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>583</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>584</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="s">
+        <v>586</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="29.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="13" t="s">
+        <v>590</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>591</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="24.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="13" t="s">
+        <v>594</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>595</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="30.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>600</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="13" t="s">
+        <v>602</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>603</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>604</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://youtu.be/KLlXCFG5TnA"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://leetcode.com/problems/two-sum/"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://youtu.be/1pkOgXD63yU"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://leetcode.com/problems/best-time-to-buy-and-sell-stock/"/>
+    <hyperlink ref="A4" r:id="rId5" display="https://youtu.be/3OamzN90kPg"/>
+    <hyperlink ref="D4" r:id="rId6" display="https://leetcode.com/problems/contains-duplicate/"/>
+    <hyperlink ref="A5" r:id="rId7" display="https://youtu.be/bNvIQI2wAjk"/>
+    <hyperlink ref="D5" r:id="rId8" display="https://leetcode.com/problems/product-of-array-except-self/"/>
+    <hyperlink ref="A6" r:id="rId9" display="https://youtu.be/5WZl3MMT0Eg"/>
+    <hyperlink ref="D6" r:id="rId10" display="https://leetcode.com/problems/maximum-subarray/"/>
+    <hyperlink ref="A7" r:id="rId11" display="https://youtu.be/lXVy6YWFcRM"/>
+    <hyperlink ref="D7" r:id="rId12" display="https://leetcode.com/problems/maximum-product-subarray/"/>
+    <hyperlink ref="A8" r:id="rId13" display="https://youtu.be/nIVW4P8b1VA"/>
+    <hyperlink ref="D8" r:id="rId14" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/"/>
+    <hyperlink ref="A9" r:id="rId15" display="https://youtu.be/U8XENwh8Oy8"/>
+    <hyperlink ref="D9" r:id="rId16" display="https://leetcode.com/problems/search-in-rotated-sorted-array/"/>
+    <hyperlink ref="A10" r:id="rId17" display="https://youtu.be/jzZsG8n2R9A"/>
+    <hyperlink ref="D10" r:id="rId18" display="https://leetcode.com/problems/3sum/"/>
+    <hyperlink ref="A11" r:id="rId19" display="https://youtu.be/UuiTKBwPgAo"/>
+    <hyperlink ref="D11" r:id="rId20" display="https://leetcode.com/problems/container-with-most-water/"/>
+    <hyperlink ref="A12" r:id="rId21" display="https://youtu.be/gVUrDV4tZfY"/>
+    <hyperlink ref="D12" r:id="rId22" display="https://leetcode.com/problems/sum-of-two-integers/"/>
+    <hyperlink ref="A13" r:id="rId23" display="https://youtu.be/5Km3utixwZs"/>
+    <hyperlink ref="D13" r:id="rId24" display="https://leetcode.com/problems/number-of-1-bits/"/>
+    <hyperlink ref="A14" r:id="rId25" display="https://youtu.be/RyBM56RIWrM"/>
+    <hyperlink ref="D14" r:id="rId26" display="https://leetcode.com/problems/counting-bits/"/>
+    <hyperlink ref="A15" r:id="rId27" display="https://youtu.be/WnPLSRLSANE"/>
+    <hyperlink ref="D15" r:id="rId28" display="https://leetcode.com/problems/missing-number/"/>
+    <hyperlink ref="A16" r:id="rId29" display="https://youtu.be/UcoN6UjAI64"/>
+    <hyperlink ref="D16" r:id="rId30" display="https://leetcode.com/problems/reverse-bits/"/>
+    <hyperlink ref="A17" r:id="rId31" display="https://youtu.be/Y0lT9Fck7qI"/>
+    <hyperlink ref="D17" r:id="rId32" display="https://leetcode.com/problems/climbing-stairs/"/>
+    <hyperlink ref="A18" r:id="rId33" display="https://youtu.be/H9bfqozjoqs"/>
+    <hyperlink ref="D18" r:id="rId34" display="https://leetcode.com/problems/coin-change/"/>
+    <hyperlink ref="A19" r:id="rId35" display="https://youtu.be/cjWnW0hdF1Y"/>
+    <hyperlink ref="D19" r:id="rId36" display="https://leetcode.com/problems/longest-increasing-subsequence/"/>
+    <hyperlink ref="A20" r:id="rId37" display="https://youtu.be/Ua0GhsJSlWM"/>
+    <hyperlink ref="D20" r:id="rId38" display="https://leetcode.com/problems/longest-common-subsequence/"/>
+    <hyperlink ref="A21" r:id="rId39" display="https://youtu.be/Sx9NNgInc3A"/>
+    <hyperlink ref="D21" r:id="rId40" display="https://leetcode.com/problems/word-break/"/>
+    <hyperlink ref="A22" r:id="rId41" display="https://youtu.be/GBKI9VSKdGg"/>
+    <hyperlink ref="D22" r:id="rId42" display="https://leetcode.com/problems/combination-sum/"/>
+    <hyperlink ref="A23" r:id="rId43" display="https://youtu.be/73r3KWiEvyk"/>
+    <hyperlink ref="D23" r:id="rId44" display="https://leetcode.com/problems/house-robber/"/>
+    <hyperlink ref="A24" r:id="rId45" display="https://youtu.be/rWAJCfYYOvM"/>
+    <hyperlink ref="D24" r:id="rId46" display="https://leetcode.com/problems/house-robber-ii/"/>
+    <hyperlink ref="A25" r:id="rId47" display="https://youtu.be/6aEyTjOwlJU"/>
+    <hyperlink ref="D25" r:id="rId48" display="https://leetcode.com/problems/decode-ways/"/>
+    <hyperlink ref="A26" r:id="rId49" display="https://youtu.be/IlEsdxuD4lY"/>
+    <hyperlink ref="D26" r:id="rId50" display="https://leetcode.com/problems/unique-paths/"/>
+    <hyperlink ref="A27" r:id="rId51" display="https://youtu.be/Yan0cv2cLy8"/>
+    <hyperlink ref="D27" r:id="rId52" display="https://leetcode.com/problems/jump-game/"/>
+    <hyperlink ref="A28" r:id="rId53" display="https://youtu.be/mQeF6bN8hMk"/>
+    <hyperlink ref="D28" r:id="rId54" display="https://leetcode.com/problems/clone-graph/"/>
+    <hyperlink ref="A29" r:id="rId55" display="https://youtu.be/EgI5nU9etnU"/>
+    <hyperlink ref="D29" r:id="rId56" display="https://leetcode.com/problems/course-schedule/"/>
+    <hyperlink ref="A30" r:id="rId57" display="https://youtu.be/s-VkcjHqkGI"/>
+    <hyperlink ref="D30" r:id="rId58" display="https://leetcode.com/problems/pacific-atlantic-water-flow/"/>
+    <hyperlink ref="A31" r:id="rId59" display="https://youtu.be/pV2kpPD66nE"/>
+    <hyperlink ref="D31" r:id="rId60" display="https://leetcode.com/problems/number-of-islands/"/>
+    <hyperlink ref="A32" r:id="rId61" display="https://youtu.be/P6RZZMu_maU"/>
+    <hyperlink ref="D32" r:id="rId62" display="https://leetcode.com/problems/longest-consecutive-sequence/"/>
+    <hyperlink ref="A33" r:id="rId63" display="https://youtu.be/6kTZYvNNyps"/>
+    <hyperlink ref="D33" r:id="rId64" display="https://leetcode.com/problems/alien-dictionary/"/>
+    <hyperlink ref="A34" r:id="rId65" display="https://youtu.be/bXsUuownnoQ"/>
+    <hyperlink ref="D34" r:id="rId66" display="https://leetcode.com/problems/graph-valid-tree/"/>
+    <hyperlink ref="A35" r:id="rId67" display="https://youtu.be/8f1XPm4WOUc"/>
+    <hyperlink ref="D35" r:id="rId68" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/"/>
+    <hyperlink ref="A36" r:id="rId69" display="https://youtu.be/A8NUOmlwOlM"/>
+    <hyperlink ref="D36" r:id="rId70" display="https://leetcode.com/problems/insert-interval/"/>
+    <hyperlink ref="A37" r:id="rId71" display="https://youtu.be/44H3cEC2fFM"/>
+    <hyperlink ref="D37" r:id="rId72" display="https://leetcode.com/problems/merge-intervals/"/>
+    <hyperlink ref="A38" r:id="rId73" display="https://youtu.be/nONCGxWoUfM"/>
+    <hyperlink ref="D38" r:id="rId74" display="https://leetcode.com/problems/non-overlapping-intervals/"/>
+    <hyperlink ref="A39" r:id="rId75" display="https://youtu.be/PaJxqZVPhbg"/>
+    <hyperlink ref="D39" r:id="rId76" display="https://leetcode.com/problems/meeting-rooms/"/>
+    <hyperlink ref="A40" r:id="rId77" display="https://youtu.be/FdzJmTCVyJU"/>
+    <hyperlink ref="D40" r:id="rId78" display="https://leetcode.com/problems/meeting-rooms-ii/"/>
+    <hyperlink ref="A41" r:id="rId79" display="https://youtu.be/G0_I-ZF0S38"/>
+    <hyperlink ref="D41" r:id="rId80" display="https://leetcode.com/problems/reverse-linked-list/"/>
+    <hyperlink ref="A42" r:id="rId81" display="https://youtu.be/gBTe7lFR3vc"/>
+    <hyperlink ref="D42" r:id="rId82" display="https://leetcode.com/problems/linked-list-cycle/"/>
+    <hyperlink ref="A43" r:id="rId83" display="https://youtu.be/XIdigk956u0"/>
+    <hyperlink ref="D43" r:id="rId84" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
+    <hyperlink ref="A44" r:id="rId85" display="https://youtu.be/q5a5OiGbT6Q"/>
+    <hyperlink ref="D44" r:id="rId86" display="https://leetcode.com/problems/merge-k-sorted-lists/"/>
+    <hyperlink ref="A45" r:id="rId87" display="https://youtu.be/XVuQxVej6y8"/>
+    <hyperlink ref="D45" r:id="rId88" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/"/>
+    <hyperlink ref="A46" r:id="rId89" display="https://youtu.be/S5bfdUTrKLM"/>
+    <hyperlink ref="D46" r:id="rId90" display="https://leetcode.com/problems/reorder-list/"/>
+    <hyperlink ref="A47" r:id="rId91" display="https://youtu.be/T41rL0L3Pnw"/>
+    <hyperlink ref="D47" r:id="rId92" display="https://leetcode.com/problems/set-matrix-zeroes/"/>
+    <hyperlink ref="A48" r:id="rId93" display="https://youtu.be/BJnMZNwUk1M"/>
+    <hyperlink ref="D48" r:id="rId94" display="https://leetcode.com/problems/spiral-matrix/"/>
+    <hyperlink ref="A49" r:id="rId95" display="https://youtu.be/fMSJSS7eO1w"/>
+    <hyperlink ref="D49" r:id="rId96" display="https://leetcode.com/problems/rotate-image/"/>
+    <hyperlink ref="A50" r:id="rId97" display="https://youtu.be/pfiQ_PS1g8E"/>
+    <hyperlink ref="D50" r:id="rId98" display="https://leetcode.com/problems/word-search/"/>
+    <hyperlink ref="A51" r:id="rId99" display="https://youtu.be/wiGpQwVHdE0"/>
+    <hyperlink ref="D51" r:id="rId100" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/"/>
+    <hyperlink ref="A52" r:id="rId101" display="https://youtu.be/gqXU1UyA8pk"/>
+    <hyperlink ref="D52" r:id="rId102" display="https://leetcode.com/problems/longest-repeating-character-replacement/"/>
+    <hyperlink ref="A53" r:id="rId103" display="https://youtu.be/jSto0O4AJbM"/>
+    <hyperlink ref="D53" r:id="rId104" display="https://leetcode.com/problems/minimum-window-substring/"/>
+    <hyperlink ref="A54" r:id="rId105" display="https://youtu.be/9UtInBqnCgA"/>
+    <hyperlink ref="D54" r:id="rId106" display="https://leetcode.com/problems/valid-anagram/"/>
+    <hyperlink ref="A55" r:id="rId107" display="https://youtu.be/vzdNOK2oB2E"/>
+    <hyperlink ref="D55" r:id="rId108" display="https://leetcode.com/problems/group-anagrams/"/>
+    <hyperlink ref="A56" r:id="rId109" display="https://youtu.be/WTzjTskDFMg"/>
+    <hyperlink ref="D56" r:id="rId110" display="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="A57" r:id="rId111" display="https://youtu.be/jJXJ16kPFWg"/>
+    <hyperlink ref="D57" r:id="rId112" display="https://leetcode.com/problems/valid-palindrome/"/>
+    <hyperlink ref="A58" r:id="rId113" display="https://youtu.be/XYQecbcd6_c"/>
+    <hyperlink ref="D58" r:id="rId114" display="https://leetcode.com/problems/longest-palindromic-substring/"/>
+    <hyperlink ref="A59" r:id="rId115" display="https://youtu.be/4RACzI5-du8"/>
+    <hyperlink ref="D59" r:id="rId116" display="https://leetcode.com/problems/palindromic-substrings/"/>
+    <hyperlink ref="A60" r:id="rId117" display="https://youtu.be/B1k_sxOSgv8"/>
+    <hyperlink ref="D60" r:id="rId118" display="https://leetcode.com/problems/encode-and-decode-strings/"/>
+    <hyperlink ref="A61" r:id="rId119" display="https://youtu.be/hTM3phVI6YQ"/>
+    <hyperlink ref="D61" r:id="rId120" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/"/>
+    <hyperlink ref="A62" r:id="rId121" display="https://youtu.be/vRbbcKXCxOw"/>
+    <hyperlink ref="D62" r:id="rId122" display="https://leetcode.com/problems/same-tree/"/>
+    <hyperlink ref="A63" r:id="rId123" display="https://youtu.be/OnSn2XEQ4MY"/>
+    <hyperlink ref="D63" r:id="rId124" display="https://leetcode.com/problems/invert-binary-tree/"/>
+    <hyperlink ref="A64" r:id="rId125" display="https://youtu.be/Hr5cWUld4vU"/>
+    <hyperlink ref="D64" r:id="rId126" display="https://leetcode.com/problems/binary-tree-maximum-path-sum/"/>
+    <hyperlink ref="A65" r:id="rId127" display="https://youtu.be/6ZnyEApgFYg"/>
+    <hyperlink ref="D65" r:id="rId128" display="https://leetcode.com/problems/binary-tree-level-order-traversal/"/>
+    <hyperlink ref="A66" r:id="rId129" display="https://youtu.be/u4JAi2JJhI8"/>
+    <hyperlink ref="D66" r:id="rId130" display="https://leetcode.com/problems/serialize-and-deserialize-binary-tree/"/>
+    <hyperlink ref="A67" r:id="rId131" display="https://youtu.be/E36O5SWp-LE"/>
+    <hyperlink ref="D67" r:id="rId132" display="https://leetcode.com/problems/subtree-of-another-tree/"/>
+    <hyperlink ref="A68" r:id="rId133" display="https://youtu.be/ihj4IQGZ2zc"/>
+    <hyperlink ref="D68" r:id="rId134" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/"/>
+    <hyperlink ref="A69" r:id="rId135" display="https://youtu.be/s6ATEkipzow"/>
+    <hyperlink ref="D69" r:id="rId136" display="https://leetcode.com/problems/validate-binary-search-tree/"/>
+    <hyperlink ref="A70" r:id="rId137" display="https://youtu.be/5LUXSvjmGCw"/>
+    <hyperlink ref="D70" r:id="rId138" display="https://leetcode.com/problems/kth-smallest-element-in-a-bst/"/>
+    <hyperlink ref="A71" r:id="rId139" display="https://youtu.be/gs2LMfuOR9k"/>
+    <hyperlink ref="D71" r:id="rId140" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/"/>
+    <hyperlink ref="A72" r:id="rId141" display="https://youtu.be/oobqoCJlHA0"/>
+    <hyperlink ref="D72" r:id="rId142" display="https://leetcode.com/problems/implement-trie-prefix-tree/"/>
+    <hyperlink ref="A73" r:id="rId143" display="https://youtu.be/BTf05gs_8iU"/>
+    <hyperlink ref="D73" r:id="rId144" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/"/>
+    <hyperlink ref="A74" r:id="rId145" display="https://youtu.be/asbcE9mZz_U"/>
+    <hyperlink ref="D74" r:id="rId146" display="https://leetcode.com/problems/word-search-ii/"/>
+    <hyperlink ref="A75" r:id="rId147" display="https://youtu.be/q5a5OiGbT6Q"/>
+    <hyperlink ref="D75" r:id="rId148" display="https://leetcode.com/problems/merge-k-sorted-lists/"/>
+    <hyperlink ref="A76" r:id="rId149" display="https://youtu.be/YPTqKIgVk-k"/>
+    <hyperlink ref="D76" r:id="rId150" display="https://leetcode.com/problems/top-k-frequent-elements/"/>
+    <hyperlink ref="A77" r:id="rId151" display="https://youtu.be/itmhHWaHupI"/>
+    <hyperlink ref="D77" r:id="rId152" display="https://leetcode.com/problems/find-median-from-data-stream/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AdkbAdd new problemsn in kbkbkbkbkbkbs in LC list:wqý`:q!
</commit_message>
<xml_diff>
--- a/leetcode/LC-list.xlsx
+++ b/leetcode/LC-list.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Jagaran" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Amazon" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="75 - blind" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Personal" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Amazon!$A$1:$E$53</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="609">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -1841,6 +1842,18 @@
   </si>
   <si>
     <t xml:space="preserve">maintain curr median, and all num greater than med in a minHeap, and all num less than med in a maxHeap, after every insertion update median depending on odd/even num of elements;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palindromic substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palindrome linked list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest palindromic subsequence</t>
   </si>
 </sst>
 </file>
@@ -2134,10 +2147,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.22"/>
@@ -6123,7 +6136,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.44"/>
@@ -8078,11 +8091,11 @@
   </sheetPr>
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.19"/>
@@ -9060,20 +9073,20 @@
         <v>533</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
+    <row r="58" s="12" customFormat="true" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11" t="s">
         <v>534</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="11" t="s">
         <v>536</v>
       </c>
     </row>
@@ -9563,4 +9576,116 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>647</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>605</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>234</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>606</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new problem in leetcode
</commit_message>
<xml_diff>
--- a/leetcode/LC-list.xlsx
+++ b/leetcode/LC-list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="618">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -1869,6 +1869,18 @@
   </si>
   <si>
     <t xml:space="preserve">Reverse Nodes in even length groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find if linked list has a circle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes (But changed linked list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the node where the circle starts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hare and Tortoise</t>
   </si>
 </sst>
 </file>
@@ -2165,7 +2177,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.26171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.22"/>
@@ -6151,7 +6163,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.26171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.44"/>
@@ -8106,8 +8118,8 @@
   </sheetPr>
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9598,15 +9610,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.16"/>
   </cols>
@@ -9740,6 +9752,43 @@
       </c>
       <c r="F8" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add leetcode problem and leetcode article
</commit_message>
<xml_diff>
--- a/leetcode/LC-list.xlsx
+++ b/leetcode/LC-list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="625">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -1887,6 +1887,21 @@
   </si>
   <si>
     <t xml:space="preserve">Merge sorted array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product of Last K numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes (brute force)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array, DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse node in k groups</t>
   </si>
 </sst>
 </file>
@@ -2194,7 +2209,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.22"/>
@@ -6180,7 +6195,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.27734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.44"/>
@@ -8135,7 +8150,7 @@
   </sheetPr>
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
     </sheetView>
   </sheetViews>
@@ -9627,10 +9642,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9842,6 +9857,34 @@
         <v>39</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>1352</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>624</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>